<commit_message>
Survey Results update and Participant Progress bug fix (#349)
* remove phase 2 from string

* bug found in previous refactor

* Update resultsTable.jsx

* targets and updated attr

* combined attr

* everything but comparisons working eval 10

* eval 10 working, evals 8 9 broke

* eval 8,9,10 working

* compare1-4

* no _count

* order

* defs

* download issue
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/SurveyResults/Survey Delegation Variables - PH2.xlsx
+++ b/dashboard-ui/src/components/SurveyResults/Survey Delegation Variables - PH2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>Variables</t>
   </si>
@@ -103,6 +103,9 @@
     <t>BX_Compare_FC1</t>
   </si>
   <si>
+    <t>BX_Compare_FC1_Percent</t>
+  </si>
+  <si>
     <t>BX_Compare_FC1_Conf</t>
   </si>
   <si>
@@ -115,6 +118,9 @@
     <t>BX_Compare_FC2</t>
   </si>
   <si>
+    <t>BX_Compare_FC2_Percent</t>
+  </si>
+  <si>
     <t>BX_Compare_FC2_Conf</t>
   </si>
   <si>
@@ -127,6 +133,9 @@
     <t>BX_Compare_FC3</t>
   </si>
   <si>
+    <t>BX_Compare_FC3_Percent</t>
+  </si>
+  <si>
     <t>BX_Compare_FC3_Conf</t>
   </si>
   <si>
@@ -214,6 +223,9 @@
     <t>The response to the first forced choice question (aligned vs baseline, or follow the previous column for Multi KDMA)</t>
   </si>
   <si>
+    <t>The response to ""For a set of future patients, you can delegate the patients to either or both of these decision-makers. In this scenario, either of these decision makers could handle 100% of this task load in a timely manner and it is not more or less efficient to divide the work between them. How would you allocate the patients between these two decision makers?" for the first forced choice</t>
+  </si>
+  <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the first forced choice</t>
   </si>
   <si>
@@ -226,6 +238,9 @@
     <t>The response to the second forced choice question (aligned vs misaligned, or follow the previous column for Multi KDMA)</t>
   </si>
   <si>
+    <t>The response to ""For a set of future patients, you can delegate the patients to either or both of these decision-makers. In this scenario, either of these decision makers could handle 100% of this task load in a timely manner and it is not more or less efficient to divide the work between them. How would you allocate the patients between these two decision makers?" for the second forced choice</t>
+  </si>
+  <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the second forced choice question</t>
   </si>
   <si>
@@ -235,13 +250,16 @@
     <t>The response to the third forced choice question (follow the previous column)</t>
   </si>
   <si>
+    <t>The response to ""For a set of future patients, you can delegate the patients to either or both of these decision-makers. In this scenario, either of these decision makers could handle 100% of this task load in a timely manner and it is not more or less efficient to divide the work between them. How would you allocate the patients between these two decision makers?" for the third forced choice</t>
+  </si>
+  <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the third forced choice question</t>
   </si>
   <si>
     <t>Levels</t>
   </si>
   <si>
-    <t>6,7</t>
+    <t>6, 7, 8</t>
   </si>
   <si>
     <r>
@@ -345,10 +363,10 @@
     <t>aligned, baseline, misaligned, high-affiliation-low-merit, low-affiliation-high-merit, low-affiliation-low-merit, high-affiliation-high-merit</t>
   </si>
   <si>
-    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), and Affiliation Focus / Merit Focus (AF-MF)</t>
-  </si>
-  <si>
-    <t>For single attribute: 0.0 - 1.0. For multi-attribute: low/low, low/high, high/low, high/high</t>
+    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Personal Safety / Affiliation Focus (PS-AF), PS, AF (Combined), and Affiliation Focus / Merit Focus (AF-MF)</t>
+  </si>
+  <si>
+    <t>For single attribute: 0.0 - 1.0. For MF/AF multi-attribute and PS/AF Combined: low/low, low/high, high/low, high/high. For PS-AF multi-attribute: Target 1, Target 2, Target 3, Target 4.</t>
   </si>
   <si>
     <t>Medic-LN, where L is a letter and N is a number</t>
@@ -735,6 +753,13 @@
       </rPr>
       <t xml:space="preserve"> 5 - Strongly Agree</t>
     </r>
+  </si>
+  <si>
+    <t>DM1 100%,
+                    DM1 75% / DM2 25%`,
+                    DM1 50% / DM2 50%`,
+                    DM1 25% / DM2 75%,
+                    DM2 100%</t>
   </si>
   <si>
     <r>
@@ -932,7 +957,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -943,12 +968,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -986,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -994,13 +1013,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1034,10 +1050,10 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4472C4"/>
@@ -1311,54 +1327,57 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="6" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="6" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="6" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="6" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="24.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="5" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="5" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="5" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="5" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="5" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="5" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="66" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="73.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1377,13 +1396,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1407,7 +1426,7 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
@@ -1476,172 +1495,190 @@
       <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="AN1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="222.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="235.5" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="AJ2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="AL2" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="133.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="141" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="P3" s="2"/>
-      <c r="Q3" s="3"/>
+      <c r="Q3" s="2"/>
       <c r="R3" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -1651,21 +1688,30 @@
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE3" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="AK3" s="2"/>
-      <c r="AL3" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
+      <c r="AN3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delegation Results Update (#389)
* uk del

* demographics only

* targets and attr

* defs

* better filter

* NaN removal

* disable graph view
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/SurveyResults/Survey Delegation Variables - PH2.xlsx
+++ b/dashboard-ui/src/components/SurveyResults/Survey Delegation Variables - PH2.xlsx
@@ -259,7 +259,7 @@
     <t>Levels</t>
   </si>
   <si>
-    <t>6, 7, 8</t>
+    <t>6, 7, 8, 9</t>
   </si>
   <si>
     <r>
@@ -363,7 +363,7 @@
     <t>aligned, baseline, misaligned, high-affiliation-low-merit, low-affiliation-high-merit, low-affiliation-low-merit, high-affiliation-high-merit</t>
   </si>
   <si>
-    <t>Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Personal Safety / Affiliation Focus (PS-AF), PS, AF (Combined), and Affiliation Focus / Merit Focus (AF-MF)</t>
+    <t>Moral Judgement (MJ), Ingroup Bias (IO), Perceived Quantity of Lives Saved (VOL), Affiliation Focus (AF), Merit Focus (MF), Personal Safety (PS), Search vs. Stay (SS), Personal Safety / Affiliation Focus (PS-AF), PS, AF (Combined), and Affiliation Focus / Merit Focus (AF-MF)</t>
   </si>
   <si>
     <t>For single attribute: 0.0 - 1.0. For MF/AF multi-attribute and PS/AF Combined: low/low, low/high, high/low, high/high. For PS-AF multi-attribute: Target 1, Target 2, Target 3, Target 4.</t>
@@ -1005,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1021,9 +1021,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1339,17 +1336,17 @@
     <col min="4" max="4" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="19.862142857142857" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
@@ -1631,7 +1628,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="141" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="195" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>80</v>
       </c>

</xml_diff>